<commit_message>
Updated with PN and TA results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB4FB5F0-1BE9-4C18-AF49-AAE3AB5BA1FA}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93CA41DE-7994-4F5F-B80F-87E52F8873F4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Type</t>
   </si>
@@ -103,6 +103,63 @@
   <si>
     <t>Simone Petilli</t>
   </si>
+  <si>
+    <t>1'17''</t>
+  </si>
+  <si>
+    <t>Primoz Roglic</t>
+  </si>
+  <si>
+    <t>Wout Van Aert</t>
+  </si>
+  <si>
+    <t>Simon Yates</t>
+  </si>
+  <si>
+    <t>Mads Pedersen</t>
+  </si>
+  <si>
+    <t>Christophe Laporte</t>
+  </si>
+  <si>
+    <t>Mathieu Burgaudeau</t>
+  </si>
+  <si>
+    <t>Luka Mezgec</t>
+  </si>
+  <si>
+    <t>Hugo Houle</t>
+  </si>
+  <si>
+    <t>Nathan Van Hooydonck</t>
+  </si>
+  <si>
+    <t>9''</t>
+  </si>
+  <si>
+    <t>Jonas Vingegaard</t>
+  </si>
+  <si>
+    <t>Damiano Caruso</t>
+  </si>
+  <si>
+    <t>Olav Kooij</t>
+  </si>
+  <si>
+    <t>Phil Bauhaus</t>
+  </si>
+  <si>
+    <t>Jai Hindley</t>
+  </si>
+  <si>
+    <t>Thymen Arensman</t>
+  </si>
+  <si>
+    <t>Xandro Meurisse</t>
+  </si>
+  <si>
+    <t>Davide Bais</t>
+  </si>
 </sst>
 </file>
 
@@ -117,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,12 +184,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,15 +200,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
   <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,10 +574,14 @@
       <c r="D2" s="1">
         <v>154</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -544,10 +596,14 @@
       <c r="D3" s="1">
         <v>167</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2160,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,11 +2225,14 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2212,17 +2271,39 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="C2" s="1">
+        <v>4871</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2237,17 +2318,39 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="C3" s="1">
+        <v>3976</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>

</xml_diff>

<commit_message>
Updated with Milano Torino results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED793E21-46E6-429E-9A35-9105C094B19D}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB7FB21-554D-4F75-906D-836ED6B0FD9C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Type</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>1''</t>
+  </si>
+  <si>
+    <t>Milano Torino</t>
+  </si>
+  <si>
+    <t>Peter Sagan</t>
+  </si>
+  <si>
+    <t>Alexander Kristoff</t>
+  </si>
+  <si>
+    <t>Mark Cavendish</t>
+  </si>
+  <si>
+    <t>Nacer Bouhanni</t>
+  </si>
+  <si>
+    <t>Michael Morkov</t>
+  </si>
+  <si>
+    <t>Max Kanter</t>
+  </si>
+  <si>
+    <t>3''</t>
   </si>
 </sst>
 </file>
@@ -619,23 +643,35 @@
         <v>55</v>
       </c>
       <c r="E4" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -2217,7 +2253,7 @@
   <dimension ref="A1:S132"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,7 +2261,7 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -2422,15 +2458,33 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2088</v>
+      </c>
+      <c r="D6" s="1">
+        <v>94</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>

</xml_diff>

<commit_message>
Updated with Milano-Sanremo results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FB7FB21-554D-4F75-906D-836ED6B0FD9C}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F560DDB-003B-428C-8344-89106DBA256E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Runtime</t>
   </si>
   <si>
-    <t>Startlist</t>
-  </si>
-  <si>
     <t>Stage Race</t>
   </si>
   <si>
@@ -183,6 +180,54 @@
   </si>
   <si>
     <t>3''</t>
+  </si>
+  <si>
+    <t>Milan Sanremo</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Classics Squad</t>
+  </si>
+  <si>
+    <t>Milano Sanremo</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Mathieu Van Der Poel</t>
+  </si>
+  <si>
+    <t>Michael Matthews</t>
+  </si>
+  <si>
+    <t>Matej Mohoric</t>
+  </si>
+  <si>
+    <t>Anthony Turgis</t>
+  </si>
+  <si>
+    <t>Jan Tratnik</t>
+  </si>
+  <si>
+    <t>Samuele Rivi</t>
+  </si>
+  <si>
+    <t>Soren Kragh Andersen</t>
+  </si>
+  <si>
+    <t>Arnaud Demare</t>
+  </si>
+  <si>
+    <t>Alessandro Tonelli</t>
+  </si>
+  <si>
+    <t>Vincenzo Albanese</t>
+  </si>
+  <si>
+    <t>5''</t>
   </si>
 </sst>
 </file>
@@ -549,12 +594,12 @@
   <dimension ref="A1:H162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
@@ -580,17 +625,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>9</v>
@@ -602,17 +649,17 @@
         <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
@@ -624,17 +671,17 @@
         <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>6</v>
@@ -646,17 +693,19 @@
         <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
@@ -668,30 +717,60 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -2252,37 +2331,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2302,10 +2384,10 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>4871</v>
@@ -2314,31 +2396,31 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -2349,10 +2431,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>3976</v>
@@ -2361,31 +2443,31 @@
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -2417,10 +2499,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>2070</v>
@@ -2429,22 +2511,22 @@
         <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -2457,9 +2539,11 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>2088</v>
@@ -2468,22 +2552,22 @@
         <v>94</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2496,16 +2580,36 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2640</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -2538,22 +2642,54 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2880</v>
+      </c>
+      <c r="D9" s="1">
+        <v>100</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>

</xml_diff>

<commit_message>
Updated with Dwars Door Vlaanderen results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F560DDB-003B-428C-8344-89106DBA256E}"/>
+  <xr:revisionPtr revIDLastSave="457" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0273C3E-8C0A-4793-92C6-00CD0EA7137E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="120">
   <si>
     <t>Type</t>
   </si>
@@ -182,9 +182,6 @@
     <t>3''</t>
   </si>
   <si>
-    <t>Milan Sanremo</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -228,6 +225,177 @@
   </si>
   <si>
     <t>5''</t>
+  </si>
+  <si>
+    <t>Catalunya</t>
+  </si>
+  <si>
+    <t>Brugge-De Panne</t>
+  </si>
+  <si>
+    <t>2''</t>
+  </si>
+  <si>
+    <t>Brugge - De Panne</t>
+  </si>
+  <si>
+    <t>Tim Merlier</t>
+  </si>
+  <si>
+    <t>Dylan Groenewegen</t>
+  </si>
+  <si>
+    <t>Max Walscheid</t>
+  </si>
+  <si>
+    <t>Jasper Stuyven</t>
+  </si>
+  <si>
+    <t>Heinrich Haussler</t>
+  </si>
+  <si>
+    <t>Simone Consonni</t>
+  </si>
+  <si>
+    <t>Arnaud De Lie</t>
+  </si>
+  <si>
+    <t>Stanislaw Aniolkowski</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Stefan Kueng</t>
+  </si>
+  <si>
+    <t>Mike Teunissen</t>
+  </si>
+  <si>
+    <t>Biniam Girmay</t>
+  </si>
+  <si>
+    <t>Tiesj Benoot</t>
+  </si>
+  <si>
+    <t>Dylan Van Baarle</t>
+  </si>
+  <si>
+    <t>Valentin Madouas</t>
+  </si>
+  <si>
+    <t>Rasmus Tiller</t>
+  </si>
+  <si>
+    <t>Michael Gogl</t>
+  </si>
+  <si>
+    <t>Gent Wevelgem</t>
+  </si>
+  <si>
+    <t>Women's Classics</t>
+  </si>
+  <si>
+    <t>2'55''</t>
+  </si>
+  <si>
+    <t>Richard Carapaz</t>
+  </si>
+  <si>
+    <t>Nairo Quintana</t>
+  </si>
+  <si>
+    <t>Joao Almeida</t>
+  </si>
+  <si>
+    <t>Ben O'Connor</t>
+  </si>
+  <si>
+    <t>Sergio Higuita</t>
+  </si>
+  <si>
+    <t>Juan Ayuso</t>
+  </si>
+  <si>
+    <t>Kaden Groves</t>
+  </si>
+  <si>
+    <t>Tobias Halland Johannessen</t>
+  </si>
+  <si>
+    <t>Ethan Vernon</t>
+  </si>
+  <si>
+    <t>Dries Van Gestel</t>
+  </si>
+  <si>
+    <t>Ivan Garcia Cortina</t>
+  </si>
+  <si>
+    <t>Arjen Livyns</t>
+  </si>
+  <si>
+    <t>Robbe Ghys</t>
+  </si>
+  <si>
+    <t>Marianne Vos</t>
+  </si>
+  <si>
+    <t>Elisa Balsamo</t>
+  </si>
+  <si>
+    <t>Emma Norsgaard</t>
+  </si>
+  <si>
+    <t>Maria Giulia Confalonieri</t>
+  </si>
+  <si>
+    <t>Susanne Andersen</t>
+  </si>
+  <si>
+    <t>Tamara Dromova</t>
+  </si>
+  <si>
+    <t>Dwars Door Vlaanderen</t>
+  </si>
+  <si>
+    <t>Tom Pidcock</t>
+  </si>
+  <si>
+    <t>Nils Politt</t>
+  </si>
+  <si>
+    <t>Kelland O'Brien</t>
+  </si>
+  <si>
+    <t>Ben Turner</t>
+  </si>
+  <si>
+    <t>Andrea Pasqualon</t>
+  </si>
+  <si>
+    <t>Victor Campenaerts</t>
+  </si>
+  <si>
+    <t>Johan Jacobs</t>
+  </si>
+  <si>
+    <t>Chiara Consonni</t>
+  </si>
+  <si>
+    <t>Elise Chabbey</t>
+  </si>
+  <si>
+    <t>Marta Bastianelli</t>
+  </si>
+  <si>
+    <t>Pfeiffer Georgi</t>
+  </si>
+  <si>
+    <t>Rachele Barbieri</t>
+  </si>
+  <si>
+    <t>Julie De Wilde</t>
   </si>
 </sst>
 </file>
@@ -591,16 +759,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H162"/>
+  <dimension ref="A1:H169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
@@ -626,10 +794,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -678,26 +846,24 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>6</v>
-      </c>
       <c r="D4" s="1">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="E4" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,19 +871,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>
@@ -729,43 +895,43 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <v>6</v>
       </c>
       <c r="D6" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C7" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>53</v>
       </c>
       <c r="E7" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -773,114 +939,268 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1">
+        <v>42</v>
+      </c>
+      <c r="E13" s="1">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2</v>
+      </c>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="1">
+        <v>12</v>
+      </c>
+      <c r="D17" s="1">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -2322,6 +2642,76 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="1"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="1"/>
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="1"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="1"/>
+      <c r="D165" s="1"/>
+      <c r="E165" s="1"/>
+      <c r="F165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="1"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="1"/>
+      <c r="E166" s="1"/>
+      <c r="F166" s="1"/>
+      <c r="G166" s="1"/>
+      <c r="H166" s="1"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2329,28 +2719,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:S132"/>
+  <dimension ref="A1:S140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="21.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2476,20 +2866,46 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5321</v>
+      </c>
+      <c r="D4" s="1">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2497,37 +2913,17 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2070</v>
-      </c>
-      <c r="D5" s="1">
-        <v>100</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="5" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2543,31 +2939,31 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>2088</v>
+        <v>2070</v>
       </c>
       <c r="D6" s="1">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -2584,31 +2980,31 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
-        <v>2640</v>
+        <v>2088</v>
       </c>
       <c r="D7" s="1">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -2621,16 +3017,36 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2640</v>
+      </c>
+      <c r="D8" s="1">
+        <v>100</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -2643,68 +3059,76 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1">
-        <v>2880</v>
+        <v>2046</v>
       </c>
       <c r="D9" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2552</v>
+      </c>
+      <c r="D10" s="1">
+        <v>98</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -2716,16 +3140,36 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2568</v>
+      </c>
+      <c r="D11" s="1">
+        <v>96</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -2737,16 +3181,36 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2669</v>
+      </c>
+      <c r="D12" s="1">
+        <v>100</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -2757,7 +3221,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2779,16 +3243,36 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1974</v>
+      </c>
+      <c r="D14" s="1">
+        <v>100</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -2800,16 +3284,36 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2046</v>
+      </c>
+      <c r="D15" s="1">
+        <v>64</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2820,7 +3324,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2842,106 +3346,266 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2880</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1855</v>
+      </c>
+      <c r="D18" s="1">
+        <v>92</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2341</v>
+      </c>
+      <c r="D19" s="1">
+        <v>98</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2361</v>
+      </c>
+      <c r="D20" s="1">
+        <v>98</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2584</v>
+      </c>
+      <c r="D21" s="1">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -5277,6 +5941,174 @@
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
     </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="K133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+      <c r="N133" s="1"/>
+      <c r="O133" s="1"/>
+      <c r="P133" s="1"/>
+      <c r="Q133" s="1"/>
+      <c r="R133" s="1"/>
+      <c r="S133" s="1"/>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="K134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
+      <c r="O134" s="1"/>
+      <c r="P134" s="1"/>
+      <c r="Q134" s="1"/>
+      <c r="R134" s="1"/>
+      <c r="S134" s="1"/>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+      <c r="R135" s="1"/>
+      <c r="S135" s="1"/>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="K136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+      <c r="N136" s="1"/>
+      <c r="O136" s="1"/>
+      <c r="P136" s="1"/>
+      <c r="Q136" s="1"/>
+      <c r="R136" s="1"/>
+      <c r="S136" s="1"/>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="K137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+      <c r="N137" s="1"/>
+      <c r="O137" s="1"/>
+      <c r="P137" s="1"/>
+      <c r="Q137" s="1"/>
+      <c r="R137" s="1"/>
+      <c r="S137" s="1"/>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="K138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+      <c r="N138" s="1"/>
+      <c r="O138" s="1"/>
+      <c r="P138" s="1"/>
+      <c r="Q138" s="1"/>
+      <c r="R138" s="1"/>
+      <c r="S138" s="1"/>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="K139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+      <c r="N139" s="1"/>
+      <c r="O139" s="1"/>
+      <c r="P139" s="1"/>
+      <c r="Q139" s="1"/>
+      <c r="R139" s="1"/>
+      <c r="S139" s="1"/>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="K140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+      <c r="N140" s="1"/>
+      <c r="O140" s="1"/>
+      <c r="P140" s="1"/>
+      <c r="Q140" s="1"/>
+      <c r="R140" s="1"/>
+      <c r="S140" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Ronde Van Vlaanderen results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="457" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0273C3E-8C0A-4793-92C6-00CD0EA7137E}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D3E91E-9769-4792-A6FA-D2AF70E5BCB5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
   <si>
     <t>Type</t>
   </si>
@@ -396,6 +396,63 @@
   </si>
   <si>
     <t>Julie De Wilde</t>
+  </si>
+  <si>
+    <t>Ronde Van Vlaanderen</t>
+  </si>
+  <si>
+    <t>Fred Wright</t>
+  </si>
+  <si>
+    <t>19''</t>
+  </si>
+  <si>
+    <t>Matis Louvel</t>
+  </si>
+  <si>
+    <t>Mathijs Paasschens</t>
+  </si>
+  <si>
+    <t>Silvan Dillier</t>
+  </si>
+  <si>
+    <t>4''</t>
+  </si>
+  <si>
+    <t>Annemiek Van Vleuten</t>
+  </si>
+  <si>
+    <t>Lotte Kopecky</t>
+  </si>
+  <si>
+    <t>Arlenis Sierra</t>
+  </si>
+  <si>
+    <t>Brodie Chapman</t>
+  </si>
+  <si>
+    <t>Silvia Persico</t>
+  </si>
+  <si>
+    <t>Chantal Van Den Broek-Blaak</t>
+  </si>
+  <si>
+    <t>Tom Bohli</t>
+  </si>
+  <si>
+    <t>Lyndsay De Wylder</t>
+  </si>
+  <si>
+    <t>Julien Vermote</t>
+  </si>
+  <si>
+    <t>Manuele Boaro</t>
+  </si>
+  <si>
+    <t>Taco Van Der Hoorn</t>
+  </si>
+  <si>
+    <t>Itzulia</t>
   </si>
 </sst>
 </file>
@@ -411,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +478,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,12 +506,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -759,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,46 +943,40 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="1">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
       <c r="D5" s="1">
-        <v>55</v>
-      </c>
-      <c r="E5" s="1">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>6</v>
       </c>
       <c r="D6" s="1">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -919,22 +988,22 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -943,22 +1012,22 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="G8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -967,19 +1036,19 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1">
         <v>2</v>
@@ -991,19 +1060,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
@@ -1015,19 +1084,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1">
         <v>6</v>
       </c>
       <c r="D11" s="1">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
@@ -1036,16 +1105,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1">
         <v>23</v>
@@ -1060,70 +1129,70 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1">
         <v>22</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G15" s="1">
         <v>2</v>
@@ -1132,25 +1201,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E16" s="1">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -1159,22 +1228,22 @@
         <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1">
         <v>12</v>
       </c>
       <c r="D17" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1183,19 +1252,19 @@
         <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1">
         <v>12</v>
       </c>
       <c r="D18" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1">
         <v>2</v>
@@ -1203,44 +1272,100 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1">
+        <v>19</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1">
+        <v>12</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1">
+        <v>21</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>54</v>
+      </c>
+      <c r="E22" s="1">
+        <v>23</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -2712,6 +2837,36 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2719,19 +2874,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:S140"/>
+  <dimension ref="A1:V142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="20.140625" customWidth="1"/>
@@ -2741,6 +2896,11 @@
     <col min="14" max="14" width="17.85546875" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3221,17 +3381,37 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3138</v>
+      </c>
+      <c r="D13" s="1">
+        <v>96</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -3242,37 +3422,17 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1974</v>
-      </c>
-      <c r="D14" s="1">
-        <v>100</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>105</v>
-      </c>
+    <row r="14" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -3288,31 +3448,31 @@
         <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1">
-        <v>2046</v>
+        <v>1974</v>
       </c>
       <c r="D15" s="1">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3324,17 +3484,37 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2046</v>
+      </c>
+      <c r="D16" s="1">
+        <v>64</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -3345,335 +3525,400 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1">
-        <v>2880</v>
+        <v>3210</v>
       </c>
       <c r="D17" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1855</v>
-      </c>
-      <c r="D18" s="1">
-        <v>92</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>74</v>
-      </c>
+    <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1">
-        <v>2341</v>
+        <v>2880</v>
       </c>
       <c r="D19" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1">
-        <v>2361</v>
+        <v>1855</v>
       </c>
       <c r="D20" s="1">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1">
-        <v>2584</v>
+        <v>2341</v>
       </c>
       <c r="D21" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="I21" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="M21" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2361</v>
+      </c>
+      <c r="D22" s="1">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2584</v>
+      </c>
+      <c r="D23" s="1">
+        <v>96</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3204</v>
+      </c>
+      <c r="D24" s="1">
+        <v>100</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3694,7 +3939,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3715,7 +3960,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3736,7 +3981,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3757,7 +4002,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3778,7 +4023,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3799,7 +4044,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3820,7 +4065,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -6109,6 +6354,48 @@
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
     </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="1"/>
+      <c r="D141" s="1"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="1"/>
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="K141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
+      <c r="O141" s="1"/>
+      <c r="P141" s="1"/>
+      <c r="Q141" s="1"/>
+      <c r="R141" s="1"/>
+      <c r="S141" s="1"/>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="1"/>
+      <c r="D142" s="1"/>
+      <c r="E142" s="1"/>
+      <c r="F142" s="1"/>
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="K142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+      <c r="N142" s="1"/>
+      <c r="O142" s="1"/>
+      <c r="P142" s="1"/>
+      <c r="Q142" s="1"/>
+      <c r="R142" s="1"/>
+      <c r="S142" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Scheldeprijs results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D3E91E-9769-4792-A6FA-D2AF70E5BCB5}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A403389-7D25-4E9A-8FB1-07D600DDE7C3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="154">
   <si>
     <t>Type</t>
   </si>
@@ -453,6 +453,51 @@
   </si>
   <si>
     <t>Itzulia</t>
+  </si>
+  <si>
+    <t>Scheldeprijs</t>
+  </si>
+  <si>
+    <t>Lorena Wiebes</t>
+  </si>
+  <si>
+    <t>Barbara Guarischi</t>
+  </si>
+  <si>
+    <t>Charlotte Kool</t>
+  </si>
+  <si>
+    <t>Georgia Baker</t>
+  </si>
+  <si>
+    <t>Danny Van Poppel</t>
+  </si>
+  <si>
+    <t>Edward Theuns</t>
+  </si>
+  <si>
+    <t>Ryan Mullen</t>
+  </si>
+  <si>
+    <t>Sam Welsford</t>
+  </si>
+  <si>
+    <t>Kenneth Vanbilsen</t>
+  </si>
+  <si>
+    <t>Jasper Philipsen</t>
+  </si>
+  <si>
+    <t>Jordi Meeus</t>
+  </si>
+  <si>
+    <t>Dan McLay</t>
+  </si>
+  <si>
+    <t>Ruediger Selig</t>
+  </si>
+  <si>
+    <t>Sam Bennett</t>
   </si>
 </sst>
 </file>
@@ -834,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1153,25 +1198,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C14" s="1">
         <v>6</v>
       </c>
       <c r="D14" s="1">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -1180,16 +1225,16 @@
         <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
       </c>
       <c r="D15" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E15" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>39</v>
@@ -1204,43 +1249,43 @@
         <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="G17" s="1">
         <v>1</v>
@@ -1249,22 +1294,22 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G18" s="1">
         <v>2</v>
@@ -1276,22 +1321,22 @@
         <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1">
         <v>12</v>
       </c>
       <c r="D19" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -1300,19 +1345,19 @@
         <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1">
         <v>12</v>
       </c>
       <c r="D20" s="1">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1">
         <v>2</v>
@@ -1324,7 +1369,7 @@
         <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1">
         <v>12</v>
@@ -1333,10 +1378,10 @@
         <v>44</v>
       </c>
       <c r="E21" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
@@ -1348,54 +1393,96 @@
         <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>12</v>
       </c>
       <c r="D22" s="1">
+        <v>55</v>
+      </c>
+      <c r="E22" s="1">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="1">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
         <v>54</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E24" s="1">
         <v>23</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G24" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="1">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1">
+        <v>41</v>
+      </c>
+      <c r="E25" s="1">
+        <v>18</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -2867,6 +2954,26 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+      <c r="D173" s="1"/>
+      <c r="E173" s="1"/>
+      <c r="F173" s="1"/>
+      <c r="G173" s="1"/>
+      <c r="H173" s="1"/>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="G174" s="1"/>
+      <c r="H174" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2874,10 +2981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V142"/>
+  <dimension ref="A1:V145"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,9 +3180,13 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -3094,37 +3205,17 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2070</v>
-      </c>
-      <c r="D6" s="1">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="6" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -3140,31 +3231,31 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
-        <v>2088</v>
+        <v>2070</v>
       </c>
       <c r="D7" s="1">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -3181,31 +3272,31 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1">
-        <v>2640</v>
+        <v>2088</v>
       </c>
       <c r="D8" s="1">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -3222,31 +3313,31 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
-        <v>2046</v>
+        <v>2640</v>
       </c>
       <c r="D9" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -3263,31 +3354,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1">
-        <v>2552</v>
+        <v>2046</v>
       </c>
       <c r="D10" s="1">
         <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -3304,31 +3395,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1">
-        <v>2568</v>
+        <v>2552</v>
       </c>
       <c r="D11" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -3345,31 +3436,31 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1">
-        <v>2669</v>
+        <v>2568</v>
       </c>
       <c r="D12" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -3386,31 +3477,31 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1">
-        <v>3138</v>
+        <v>2669</v>
       </c>
       <c r="D13" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -3422,17 +3513,37 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3138</v>
+      </c>
+      <c r="D14" s="1">
+        <v>96</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -3445,34 +3556,34 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1">
-        <v>1974</v>
+        <v>2034</v>
       </c>
       <c r="D15" s="1">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3484,37 +3595,17 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1">
-        <v>2046</v>
-      </c>
-      <c r="D16" s="1">
-        <v>64</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>119</v>
-      </c>
+    <row r="16" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -3530,31 +3621,31 @@
         <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1">
-        <v>3210</v>
+        <v>1974</v>
       </c>
       <c r="D17" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -3566,17 +3657,37 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2046</v>
+      </c>
+      <c r="D18" s="1">
+        <v>64</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -3589,159 +3700,103 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1">
-        <v>2880</v>
+        <v>3210</v>
       </c>
       <c r="D19" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>55</v>
+        <v>130</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
       <c r="C20" s="1">
-        <v>1855</v>
+        <v>2052</v>
       </c>
       <c r="D20" s="1">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>68</v>
+        <v>141</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2341</v>
-      </c>
-      <c r="D21" s="1">
-        <v>98</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>83</v>
-      </c>
+    <row r="21" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -3751,49 +3806,49 @@
         <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>2361</v>
+        <v>2880</v>
       </c>
       <c r="D22" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
@@ -3804,49 +3859,49 @@
         <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1">
-        <v>2584</v>
+        <v>1855</v>
       </c>
       <c r="D23" s="1">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
@@ -3857,147 +3912,275 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1">
-        <v>3204</v>
+        <v>2341</v>
       </c>
       <c r="D24" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2361</v>
+      </c>
+      <c r="D25" s="1">
+        <v>98</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2584</v>
+      </c>
+      <c r="D26" s="1">
+        <v>96</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3204</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
+      <c r="R27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3565</v>
+      </c>
+      <c r="D28" s="1">
+        <v>86</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -6396,6 +6579,69 @@
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
     </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="K143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
+      <c r="O143" s="1"/>
+      <c r="P143" s="1"/>
+      <c r="Q143" s="1"/>
+      <c r="R143" s="1"/>
+      <c r="S143" s="1"/>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="K144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+      <c r="N144" s="1"/>
+      <c r="O144" s="1"/>
+      <c r="P144" s="1"/>
+      <c r="Q144" s="1"/>
+      <c r="R144" s="1"/>
+      <c r="S144" s="1"/>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1"/>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="K145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1"/>
+      <c r="N145" s="1"/>
+      <c r="O145" s="1"/>
+      <c r="P145" s="1"/>
+      <c r="Q145" s="1"/>
+      <c r="R145" s="1"/>
+      <c r="S145" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Amstel Gold Race results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="617" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A403389-7D25-4E9A-8FB1-07D600DDE7C3}"/>
+  <xr:revisionPtr revIDLastSave="706" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A6DDEB-C224-4F8B-BB90-678E618645C7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="175">
   <si>
     <t>Type</t>
   </si>
@@ -416,9 +416,6 @@
     <t>Silvan Dillier</t>
   </si>
   <si>
-    <t>4''</t>
-  </si>
-  <si>
     <t>Annemiek Van Vleuten</t>
   </si>
   <si>
@@ -498,6 +495,72 @@
   </si>
   <si>
     <t>Sam Bennett</t>
+  </si>
+  <si>
+    <t>Dani Martinez</t>
+  </si>
+  <si>
+    <t>Remco Evenepoel</t>
+  </si>
+  <si>
+    <t>Aleksandr Vlasov</t>
+  </si>
+  <si>
+    <t>Pello Bilbao</t>
+  </si>
+  <si>
+    <t>Ion Izagirre</t>
+  </si>
+  <si>
+    <t>Carlos Rodriguez</t>
+  </si>
+  <si>
+    <t>Felix Gall</t>
+  </si>
+  <si>
+    <t>Orluis Aular</t>
+  </si>
+  <si>
+    <t>Fabien Doubey</t>
+  </si>
+  <si>
+    <t>Amstel Gold Race</t>
+  </si>
+  <si>
+    <t>Demi Vollering</t>
+  </si>
+  <si>
+    <t>Marta Cavalli</t>
+  </si>
+  <si>
+    <t>Liane Lippert</t>
+  </si>
+  <si>
+    <t>Alexandra Manly</t>
+  </si>
+  <si>
+    <t>Elizabeth Holden</t>
+  </si>
+  <si>
+    <t>Benoit Cosnefroy</t>
+  </si>
+  <si>
+    <t>Michal Kwiatkowski</t>
+  </si>
+  <si>
+    <t>Alexander Kamp</t>
+  </si>
+  <si>
+    <t>Marc Hirschi</t>
+  </si>
+  <si>
+    <t>Aaron Van Poucke</t>
+  </si>
+  <si>
+    <t>Jan Tartnik</t>
+  </si>
+  <si>
+    <t>Owain Doull</t>
   </si>
 </sst>
 </file>
@@ -513,7 +576,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,12 +592,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1048,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1">
         <v>9</v>
@@ -999,10 +1056,14 @@
       <c r="D5" s="1">
         <v>155</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1201,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="1">
         <v>6</v>
@@ -1222,19 +1283,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
       </c>
       <c r="D15" s="1">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>39</v>
@@ -1249,16 +1310,16 @@
         <v>85</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
@@ -1273,22 +1334,22 @@
         <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>126</v>
+        <v>39</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1297,70 +1358,70 @@
         <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="C19" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C20" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1">
-        <v>22</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1369,22 +1430,22 @@
         <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1">
         <v>12</v>
       </c>
       <c r="D21" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E21" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1393,19 +1454,19 @@
         <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
@@ -1417,7 +1478,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1">
         <v>12</v>
@@ -1426,10 +1487,10 @@
         <v>44</v>
       </c>
       <c r="E23" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
@@ -1441,22 +1502,22 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1">
         <v>12</v>
       </c>
       <c r="D24" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E24" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1465,19 +1526,19 @@
         <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1">
         <v>12</v>
       </c>
       <c r="D25" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E25" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G25" s="1">
         <v>2</v>
@@ -1485,34 +1546,76 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="1">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1">
+        <v>23</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="1">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1">
+        <v>18</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="1">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1">
+        <v>49</v>
+      </c>
+      <c r="E28" s="1">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
@@ -2974,6 +3077,26 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
     </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+      <c r="D175" s="1"/>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="1"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2981,18 +3104,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V145"/>
+  <dimension ref="A1:V147"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
@@ -3185,19 +3307,41 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4549</v>
+      </c>
+      <c r="D5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -3559,7 +3703,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1">
         <v>2034</v>
@@ -3571,19 +3715,19 @@
         <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -3595,17 +3739,37 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2106</v>
+      </c>
+      <c r="D16" s="1">
+        <v>100</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -3616,37 +3780,17 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1974</v>
-      </c>
-      <c r="D17" s="1">
-        <v>100</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>105</v>
-      </c>
+    <row r="17" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -3662,31 +3806,31 @@
         <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1">
-        <v>2046</v>
+        <v>1974</v>
       </c>
       <c r="D18" s="1">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -3703,31 +3847,31 @@
         <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1">
-        <v>3210</v>
+        <v>2046</v>
       </c>
       <c r="D19" s="1">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -3744,31 +3888,31 @@
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1">
-        <v>2052</v>
+        <v>3210</v>
       </c>
       <c r="D20" s="1">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -3780,17 +3924,37 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2052</v>
+      </c>
+      <c r="D21" s="1">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -3803,106 +3967,62 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="C22" s="1">
-        <v>2880</v>
+        <v>2544</v>
       </c>
       <c r="D22" s="1">
         <v>100</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1855</v>
-      </c>
-      <c r="D23" s="1">
-        <v>92</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>74</v>
-      </c>
+    <row r="23" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -3912,49 +4032,49 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1">
-        <v>2341</v>
+        <v>2880</v>
       </c>
       <c r="D24" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
@@ -3965,49 +4085,49 @@
         <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C25" s="1">
-        <v>2361</v>
+        <v>1855</v>
       </c>
       <c r="D25" s="1">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -4018,49 +4138,49 @@
         <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1">
-        <v>2584</v>
+        <v>2341</v>
       </c>
       <c r="D26" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="I26" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="M26" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
@@ -4071,179 +4191,275 @@
         <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C27" s="1">
-        <v>3204</v>
+        <v>2361</v>
       </c>
       <c r="D27" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>125</v>
+        <v>96</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="U27" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="V27" s="3" t="s">
-        <v>137</v>
-      </c>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="C28" s="1">
-        <v>3565</v>
+        <v>2584</v>
       </c>
       <c r="D28" s="1">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3204</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
+      <c r="R29" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V29" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3565</v>
+      </c>
+      <c r="D30" s="1">
+        <v>86</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2780</v>
+      </c>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -6642,6 +6858,48 @@
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
     </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="1"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="K146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+      <c r="N146" s="1"/>
+      <c r="O146" s="1"/>
+      <c r="P146" s="1"/>
+      <c r="Q146" s="1"/>
+      <c r="R146" s="1"/>
+      <c r="S146" s="1"/>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="K147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="M147" s="1"/>
+      <c r="N147" s="1"/>
+      <c r="O147" s="1"/>
+      <c r="P147" s="1"/>
+      <c r="Q147" s="1"/>
+      <c r="R147" s="1"/>
+      <c r="S147" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with BP and PR results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22A6DDEB-C224-4F8B-BB90-678E618645C7}"/>
+  <xr:revisionPtr revIDLastSave="840" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{052098C2-599C-4459-B2C6-54CB5592A56D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="195">
   <si>
     <t>Type</t>
   </si>
@@ -561,6 +561,66 @@
   </si>
   <si>
     <t>Owain Doull</t>
+  </si>
+  <si>
+    <t>Brabantse Pijl</t>
+  </si>
+  <si>
+    <t>Katarzyna Niewiadoma</t>
+  </si>
+  <si>
+    <t>Marlen Reusser</t>
+  </si>
+  <si>
+    <t>Pauliena Rooijakkers</t>
+  </si>
+  <si>
+    <t>Warren Barguil</t>
+  </si>
+  <si>
+    <t>Tim Wellens</t>
+  </si>
+  <si>
+    <t>Magnus Sheffield</t>
+  </si>
+  <si>
+    <t>Dylan Teuns</t>
+  </si>
+  <si>
+    <t>Michael Valgren</t>
+  </si>
+  <si>
+    <t>Dorian Godon</t>
+  </si>
+  <si>
+    <t>Laurens De Plus</t>
+  </si>
+  <si>
+    <t>Paris Roubaix</t>
+  </si>
+  <si>
+    <t>Elisa Longo Borghini</t>
+  </si>
+  <si>
+    <t>Lucinda Brand</t>
+  </si>
+  <si>
+    <t>Ellen Van Dijk</t>
+  </si>
+  <si>
+    <t>Victoire Berteau</t>
+  </si>
+  <si>
+    <t>Tom Devriendt</t>
+  </si>
+  <si>
+    <t>Laurent Pichon</t>
+  </si>
+  <si>
+    <t>Yves Lampaert</t>
+  </si>
+  <si>
+    <t>Adrien Petit</t>
   </si>
 </sst>
 </file>
@@ -936,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,49 +1367,49 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>175</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E16" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E17" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1358,22 +1418,22 @@
         <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1">
-        <v>17</v>
-      </c>
-      <c r="F18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -1382,7 +1442,7 @@
         <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C19" s="1">
         <v>6</v>
@@ -1391,7 +1451,7 @@
         <v>42</v>
       </c>
       <c r="E19" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -1406,16 +1466,16 @@
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C20" s="1">
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E20" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>39</v>
@@ -1427,70 +1487,70 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="C21" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="C22" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E22" s="1">
-        <v>22</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="C23" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1">
-        <v>19</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
@@ -1499,25 +1559,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="C24" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1">
-        <v>19</v>
-      </c>
-      <c r="F24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1526,13 +1586,13 @@
         <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1">
         <v>12</v>
       </c>
       <c r="D25" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E25" s="1">
         <v>21</v>
@@ -1541,7 +1601,7 @@
         <v>62</v>
       </c>
       <c r="G25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1550,22 +1610,22 @@
         <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1">
         <v>12</v>
       </c>
       <c r="D26" s="1">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="G26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1574,19 +1634,19 @@
         <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1">
         <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E27" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G27" s="1">
         <v>2</v>
@@ -1598,84 +1658,168 @@
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C28" s="1">
         <v>12</v>
       </c>
       <c r="D28" s="1">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1">
+        <v>19</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="1">
+      <c r="B29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="1">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44</v>
+      </c>
+      <c r="E29" s="1">
+        <v>21</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="1">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1">
+        <v>54</v>
+      </c>
+      <c r="E30" s="1">
+        <v>23</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="1">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1">
+        <v>41</v>
+      </c>
+      <c r="E31" s="1">
+        <v>18</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="1">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1">
+        <v>49</v>
+      </c>
+      <c r="E32" s="1">
         <v>20</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G32" s="1">
         <v>1</v>
       </c>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="1">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1">
+        <v>48</v>
+      </c>
+      <c r="E33" s="1">
+        <v>19</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2</v>
+      </c>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="1">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45</v>
+      </c>
+      <c r="E34" s="1">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -3097,6 +3241,46 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="1"/>
+      <c r="E177" s="1"/>
+      <c r="F177" s="1"/>
+      <c r="G177" s="1"/>
+      <c r="H177" s="1"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="1"/>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+      <c r="H178" s="1"/>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
+      <c r="F179" s="1"/>
+      <c r="G179" s="1"/>
+      <c r="H179" s="1"/>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+      <c r="E180" s="1"/>
+      <c r="F180" s="1"/>
+      <c r="G180" s="1"/>
+      <c r="H180" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3104,10 +3288,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V147"/>
+  <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3301,7 @@
     <col min="5" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
@@ -3780,17 +3964,37 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1938</v>
+      </c>
+      <c r="D17" s="1">
+        <v>92</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -3801,36 +4005,36 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="C18" s="1">
-        <v>1974</v>
+        <v>3105</v>
       </c>
       <c r="D18" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -3842,37 +4046,17 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2046</v>
-      </c>
-      <c r="D19" s="1">
-        <v>64</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>119</v>
-      </c>
+    <row r="19" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -3883,36 +4067,36 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1">
-        <v>3210</v>
+        <v>1974</v>
       </c>
       <c r="D20" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -3924,36 +4108,36 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1">
-        <v>2052</v>
+        <v>2046</v>
       </c>
       <c r="D21" s="1">
         <v>64</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>118</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -3965,36 +4149,36 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C22" s="1">
-        <v>2544</v>
+        <v>3210</v>
       </c>
       <c r="D22" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -4006,17 +4190,37 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2052</v>
+      </c>
+      <c r="D23" s="1">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -4027,570 +4231,694 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="C24" s="1">
-        <v>2880</v>
+        <v>2544</v>
       </c>
       <c r="D24" s="1">
         <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>175</v>
       </c>
       <c r="C25" s="1">
-        <v>1855</v>
+        <v>2284</v>
       </c>
       <c r="D25" s="1">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>176</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>68</v>
+        <v>177</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>69</v>
+        <v>178</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>186</v>
       </c>
       <c r="C26" s="1">
-        <v>2341</v>
+        <v>2928</v>
       </c>
       <c r="D26" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>187</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>54</v>
+        <v>188</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2361</v>
-      </c>
-      <c r="D27" s="1">
-        <v>98</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>99</v>
-      </c>
+    <row r="27" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="C28" s="1">
-        <v>2584</v>
+        <v>2880</v>
       </c>
       <c r="D28" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>56</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1">
-        <v>3204</v>
+        <v>1855</v>
       </c>
       <c r="D29" s="1">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>125</v>
+        <v>73</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="Q29" s="1"/>
-      <c r="R29" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U29" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="V29" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1">
-        <v>3565</v>
+        <v>2341</v>
       </c>
       <c r="D30" s="1">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>148</v>
+        <v>76</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>149</v>
+        <v>77</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>151</v>
+        <v>83</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C31" s="1">
-        <v>2780</v>
+        <v>2361</v>
       </c>
       <c r="D31" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>171</v>
+        <v>78</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>169</v>
+        <v>58</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>173</v>
+        <v>96</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2584</v>
+      </c>
+      <c r="D32" s="1">
+        <v>96</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3204</v>
+      </c>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P33" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="R33" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S33" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U33" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V33" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3565</v>
+      </c>
+      <c r="D34" s="1">
+        <v>86</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2780</v>
+      </c>
+      <c r="D35" s="1">
+        <v>100</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>174</v>
+      </c>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2683</v>
+      </c>
+      <c r="D36" s="1">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="1">
+        <v>3170</v>
+      </c>
+      <c r="D37" s="1">
+        <v>98</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -4611,7 +4939,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -4632,7 +4960,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4653,7 +4981,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4674,7 +5002,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -4695,7 +5023,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4716,7 +5044,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4737,7 +5065,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4758,7 +5086,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4779,7 +5107,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4800,7 +5128,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -6900,6 +7228,90 @@
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
     </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+      <c r="J148" s="1"/>
+      <c r="K148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+      <c r="N148" s="1"/>
+      <c r="O148" s="1"/>
+      <c r="P148" s="1"/>
+      <c r="Q148" s="1"/>
+      <c r="R148" s="1"/>
+      <c r="S148" s="1"/>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="K149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="M149" s="1"/>
+      <c r="N149" s="1"/>
+      <c r="O149" s="1"/>
+      <c r="P149" s="1"/>
+      <c r="Q149" s="1"/>
+      <c r="R149" s="1"/>
+      <c r="S149" s="1"/>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+      <c r="R151" s="1"/>
+      <c r="S151" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Fleche Wallonne results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="840" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{052098C2-599C-4459-B2C6-54CB5592A56D}"/>
+  <xr:revisionPtr revIDLastSave="914" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D4099A-26BA-4432-B103-C0DBEE56BF76}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="208">
   <si>
     <t>Type</t>
   </si>
@@ -621,6 +621,45 @@
   </si>
   <si>
     <t>Adrien Petit</t>
+  </si>
+  <si>
+    <t>Fleche Wallonne</t>
+  </si>
+  <si>
+    <t>Anouska Koster</t>
+  </si>
+  <si>
+    <t>Yara Kastelijn</t>
+  </si>
+  <si>
+    <t>Kristabel Doebel-Hickok</t>
+  </si>
+  <si>
+    <t>Rudy Molard</t>
+  </si>
+  <si>
+    <t>Ruben Guerreiro</t>
+  </si>
+  <si>
+    <t>22'</t>
+  </si>
+  <si>
+    <t>Julian Alaphilippe</t>
+  </si>
+  <si>
+    <t>Mike Woods</t>
+  </si>
+  <si>
+    <t>Valentin Ferron</t>
+  </si>
+  <si>
+    <t>Bruno Armirail</t>
+  </si>
+  <si>
+    <t>Jimmy Janssens</t>
+  </si>
+  <si>
+    <t>Simon Guglielmi</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H180"/>
+  <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,16 +1454,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1">
         <v>23</v>
@@ -1442,16 +1481,16 @@
         <v>85</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1">
         <v>6</v>
       </c>
       <c r="D19" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E19" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -1466,22 +1505,22 @@
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1">
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1">
-        <v>17</v>
-      </c>
-      <c r="F20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1490,22 +1529,22 @@
         <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1">
-        <v>18</v>
-      </c>
-      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1514,22 +1553,22 @@
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C22" s="1">
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
-        <v>23</v>
-      </c>
-      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -1538,13 +1577,13 @@
         <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E23" s="1">
         <v>23</v>
@@ -1553,7 +1592,7 @@
         <v>39</v>
       </c>
       <c r="G23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -1562,43 +1601,43 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E24" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="C25" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D25" s="1">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1">
-        <v>21</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>62</v>
+        <v>20</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -1607,25 +1646,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="C26" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1">
-        <v>22</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1634,22 +1673,22 @@
         <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1">
         <v>12</v>
       </c>
       <c r="D27" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E27" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -1658,19 +1697,19 @@
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
         <v>12</v>
       </c>
       <c r="D28" s="1">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G28" s="1">
         <v>2</v>
@@ -1682,7 +1721,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1">
         <v>12</v>
@@ -1691,10 +1730,10 @@
         <v>44</v>
       </c>
       <c r="E29" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G29" s="1">
         <v>2</v>
@@ -1706,22 +1745,22 @@
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1">
         <v>12</v>
       </c>
       <c r="D30" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E30" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="G30" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1730,19 +1769,19 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C31" s="1">
         <v>12</v>
       </c>
       <c r="D31" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E31" s="1">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G31" s="1">
         <v>2</v>
@@ -1754,19 +1793,19 @@
         <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1">
         <v>12</v>
       </c>
       <c r="D32" s="1">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -1778,16 +1817,16 @@
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C33" s="1">
         <v>12</v>
       </c>
       <c r="D33" s="1">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E33" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>39</v>
@@ -1802,19 +1841,19 @@
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="C34" s="1">
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E34" s="1">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -1822,34 +1861,76 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="1">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2</v>
+      </c>
+      <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C36" s="1">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1">
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="1">
+        <v>12</v>
+      </c>
+      <c r="D37" s="1">
+        <v>57</v>
+      </c>
+      <c r="E37" s="1">
+        <v>23</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2</v>
+      </c>
+      <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -3281,6 +3362,26 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+      <c r="F181" s="1"/>
+      <c r="G181" s="1"/>
+      <c r="H181" s="1"/>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
+      <c r="F182" s="1"/>
+      <c r="G182" s="1"/>
+      <c r="H182" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3288,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V151"/>
+  <dimension ref="A1:V153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,14 +3403,14 @@
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
     <col min="13" max="13" width="21.7109375" customWidth="1"/>
     <col min="14" max="14" width="17.85546875" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
     <col min="19" max="19" width="17.5703125" customWidth="1"/>
     <col min="20" max="20" width="14.28515625" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
@@ -4046,17 +4147,37 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1929</v>
+      </c>
+      <c r="D19" s="1">
+        <v>98</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -4067,37 +4188,17 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1974</v>
-      </c>
-      <c r="D20" s="1">
-        <v>100</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>105</v>
-      </c>
+    <row r="20" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -4113,31 +4214,31 @@
         <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1">
-        <v>2046</v>
+        <v>1974</v>
       </c>
       <c r="D21" s="1">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -4154,31 +4255,31 @@
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1">
-        <v>3210</v>
+        <v>2046</v>
       </c>
       <c r="D22" s="1">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -4195,31 +4296,31 @@
         <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1">
-        <v>2052</v>
+        <v>3210</v>
       </c>
       <c r="D23" s="1">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -4236,31 +4337,31 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C24" s="1">
-        <v>2544</v>
+        <v>2052</v>
       </c>
       <c r="D24" s="1">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -4277,31 +4378,31 @@
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C25" s="1">
-        <v>2284</v>
+        <v>2544</v>
       </c>
       <c r="D25" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>163</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>165</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -4318,31 +4419,31 @@
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C26" s="1">
-        <v>2928</v>
+        <v>2284</v>
       </c>
       <c r="D26" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -4354,17 +4455,37 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2928</v>
+      </c>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -4377,106 +4498,62 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1">
-        <v>2880</v>
+        <v>3039</v>
       </c>
       <c r="D28" s="1">
         <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>55</v>
+        <v>197</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1855</v>
-      </c>
-      <c r="D29" s="1">
-        <v>92</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>74</v>
-      </c>
+    <row r="29" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -4486,49 +4563,49 @@
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1">
-        <v>2341</v>
+        <v>2880</v>
       </c>
       <c r="D30" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="I30" s="1" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
@@ -4539,49 +4616,49 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1">
-        <v>2361</v>
+        <v>1855</v>
       </c>
       <c r="D31" s="1">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
@@ -4592,49 +4669,49 @@
         <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1">
-        <v>2584</v>
+        <v>2341</v>
       </c>
       <c r="D32" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="G32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="I32" s="1" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="J32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="M32" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -4645,115 +4722,102 @@
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C33" s="1">
-        <v>3204</v>
+        <v>2361</v>
       </c>
       <c r="D33" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P33" s="3" t="s">
-        <v>125</v>
+        <v>96</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="Q33" s="1"/>
-      <c r="R33" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S33" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T33" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U33" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="V33" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1">
-        <v>3565</v>
+        <v>2584</v>
       </c>
       <c r="D34" s="1">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -4764,102 +4828,115 @@
         <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1">
-        <v>2780</v>
+        <v>3204</v>
       </c>
       <c r="D35" s="1">
         <v>100</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G35" s="1" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>172</v>
+        <v>56</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>174</v>
+        <v>123</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
+      <c r="R35" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T35" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1">
-        <v>2683</v>
+        <v>3565</v>
       </c>
       <c r="D36" s="1">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>168</v>
+        <v>67</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>37</v>
+        <v>150</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -4870,115 +4947,213 @@
         <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="C37" s="1">
-        <v>3170</v>
+        <v>2780</v>
       </c>
       <c r="D37" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2683</v>
+      </c>
+      <c r="D38" s="1">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3170</v>
+      </c>
+      <c r="D39" s="1">
+        <v>98</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1910</v>
+      </c>
+      <c r="D40" s="1">
+        <v>100</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="R40" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
@@ -7312,6 +7487,48 @@
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
     </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="K152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+      <c r="N152" s="1"/>
+      <c r="O152" s="1"/>
+      <c r="P152" s="1"/>
+      <c r="Q152" s="1"/>
+      <c r="R152" s="1"/>
+      <c r="S152" s="1"/>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="K153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+      <c r="N153" s="1"/>
+      <c r="O153" s="1"/>
+      <c r="P153" s="1"/>
+      <c r="Q153" s="1"/>
+      <c r="R153" s="1"/>
+      <c r="S153" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Liege Bastogne Liege results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="914" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D4099A-26BA-4432-B103-C0DBEE56BF76}"/>
+  <xr:revisionPtr revIDLastSave="1003" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D570B59-419E-49CF-880E-C95344950288}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="223">
   <si>
     <t>Type</t>
   </si>
@@ -660,6 +660,51 @@
   </si>
   <si>
     <t>Simon Guglielmi</t>
+  </si>
+  <si>
+    <t>Liege Bastogne Liege</t>
+  </si>
+  <si>
+    <t>Grace Brown</t>
+  </si>
+  <si>
+    <t>15''</t>
+  </si>
+  <si>
+    <t>Neilson Powless</t>
+  </si>
+  <si>
+    <t>Quinten Hermans</t>
+  </si>
+  <si>
+    <t>Sergio Hiuita</t>
+  </si>
+  <si>
+    <t>Sylvain Moniquet</t>
+  </si>
+  <si>
+    <t>Luc Wirtgen</t>
+  </si>
+  <si>
+    <t>Paul Ourselin</t>
+  </si>
+  <si>
+    <t>Ultimate Squad</t>
+  </si>
+  <si>
+    <t>No Subs</t>
+  </si>
+  <si>
+    <t>12x12</t>
+  </si>
+  <si>
+    <t>Thirty Subs</t>
+  </si>
+  <si>
+    <t>73/94</t>
+  </si>
+  <si>
+    <t>Romandie</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,46 +1211,38 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="1">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1">
-        <v>55</v>
-      </c>
-      <c r="E6" s="1">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E7" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1">
         <v>2</v>
@@ -1217,22 +1254,22 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -1241,22 +1278,22 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="G9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -1265,19 +1302,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
@@ -1289,19 +1326,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1">
         <v>6</v>
       </c>
       <c r="D11" s="1">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
@@ -1313,19 +1350,19 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" s="1">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
@@ -1337,22 +1374,22 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
       </c>
       <c r="D13" s="1">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2"/>
     </row>
@@ -1361,22 +1398,22 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1">
         <v>6</v>
       </c>
       <c r="D14" s="1">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -1385,13 +1422,13 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
       </c>
       <c r="D15" s="1">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1">
         <v>17</v>
@@ -1400,7 +1437,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H15" s="2"/>
     </row>
@@ -1409,13 +1446,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1">
         <v>17</v>
@@ -1424,7 +1461,7 @@
         <v>39</v>
       </c>
       <c r="G16" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -1433,22 +1470,22 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1457,37 +1494,37 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E18" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="C19" s="1">
         <v>6</v>
       </c>
       <c r="D19" s="1">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1">
         <v>23</v>
@@ -1502,25 +1539,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>106</v>
+        <v>208</v>
       </c>
       <c r="C20" s="1">
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>210</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1529,22 +1566,22 @@
         <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E21" s="1">
-        <v>17</v>
-      </c>
-      <c r="F21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1553,7 +1590,7 @@
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C22" s="1">
         <v>6</v>
@@ -1562,7 +1599,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>39</v>
@@ -1577,16 +1614,16 @@
         <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E23" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>39</v>
@@ -1601,18 +1638,18 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E24" s="1">
-        <v>23</v>
-      </c>
-      <c r="F24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="1">
@@ -1625,16 +1662,16 @@
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
       </c>
       <c r="D25" s="1">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E25" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>39</v>
@@ -1649,13 +1686,13 @@
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C26" s="1">
         <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E26" s="1">
         <v>23</v>
@@ -1664,28 +1701,28 @@
         <v>39</v>
       </c>
       <c r="G26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="C27" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D27" s="1">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1">
-        <v>21</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>62</v>
+        <v>20</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -1694,49 +1731,49 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1">
-        <v>22</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="G28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>208</v>
       </c>
       <c r="C29" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" s="1">
-        <v>19</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="G29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -1745,22 +1782,22 @@
         <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1">
         <v>12</v>
       </c>
       <c r="D30" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="G30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1769,19 +1806,19 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1">
         <v>12</v>
       </c>
       <c r="D31" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E31" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="G31" s="1">
         <v>2</v>
@@ -1793,22 +1830,22 @@
         <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1">
         <v>12</v>
       </c>
       <c r="D32" s="1">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E32" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>122</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -1817,16 +1854,16 @@
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="C33" s="1">
         <v>12</v>
       </c>
       <c r="D33" s="1">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E33" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>39</v>
@@ -1841,22 +1878,22 @@
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="C34" s="1">
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E34" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -1865,22 +1902,22 @@
         <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
       <c r="C35" s="1">
         <v>12</v>
       </c>
       <c r="D35" s="1">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E35" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="G35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -1889,22 +1926,22 @@
         <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1">
         <v>12</v>
       </c>
       <c r="D36" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E36" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -1913,84 +1950,160 @@
         <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="C37" s="1">
         <v>12</v>
       </c>
       <c r="D37" s="1">
+        <v>49</v>
+      </c>
+      <c r="E37" s="1">
+        <v>20</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="1">
+        <v>12</v>
+      </c>
+      <c r="D38" s="1">
+        <v>48</v>
+      </c>
+      <c r="E38" s="1">
+        <v>19</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="1">
+        <v>12</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45</v>
+      </c>
+      <c r="E39" s="1">
+        <v>15</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="1">
+        <v>12</v>
+      </c>
+      <c r="D40" s="1">
         <v>57</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E40" s="1">
         <v>23</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G40" s="1">
         <v>2</v>
       </c>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="1">
+        <v>12</v>
+      </c>
+      <c r="D41" s="1">
+        <v>54</v>
+      </c>
+      <c r="E41" s="1">
+        <v>25</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D42" s="1">
+        <v>312</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="1">
+        <v>312</v>
+      </c>
+      <c r="E43" s="1">
+        <v>94</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -3382,6 +3495,36 @@
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="1"/>
+      <c r="F183" s="1"/>
+      <c r="G183" s="1"/>
+      <c r="H183" s="1"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="1"/>
+      <c r="E184" s="1"/>
+      <c r="F184" s="1"/>
+      <c r="G184" s="1"/>
+      <c r="H184" s="1"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
+      <c r="E185" s="1"/>
+      <c r="F185" s="1"/>
+      <c r="G185" s="1"/>
+      <c r="H185" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3389,10 +3532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V153"/>
+  <dimension ref="A1:V156"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,9 +3777,13 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3655,37 +3802,17 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2070</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="7" spans="1:19" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -3701,31 +3828,31 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>2088</v>
+        <v>2070</v>
       </c>
       <c r="D8" s="1">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -3742,31 +3869,31 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
-        <v>2640</v>
+        <v>2088</v>
       </c>
       <c r="D9" s="1">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -3783,31 +3910,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1">
-        <v>2046</v>
+        <v>2640</v>
       </c>
       <c r="D10" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -3824,31 +3951,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1">
-        <v>2552</v>
+        <v>2046</v>
       </c>
       <c r="D11" s="1">
         <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -3865,31 +3992,31 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1">
-        <v>2568</v>
+        <v>2552</v>
       </c>
       <c r="D12" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -3906,31 +4033,31 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C13" s="1">
-        <v>2669</v>
+        <v>2568</v>
       </c>
       <c r="D13" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -3947,31 +4074,31 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1">
-        <v>3138</v>
+        <v>2669</v>
       </c>
       <c r="D14" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -3988,31 +4115,31 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C15" s="1">
-        <v>2034</v>
+        <v>3138</v>
       </c>
       <c r="D15" s="1">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -4029,31 +4156,31 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C16" s="1">
-        <v>2106</v>
+        <v>2034</v>
       </c>
       <c r="D16" s="1">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -4070,31 +4197,31 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C17" s="1">
-        <v>1938</v>
+        <v>2106</v>
       </c>
       <c r="D17" s="1">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>168</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>179</v>
+        <v>79</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -4111,31 +4238,31 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C18" s="1">
-        <v>3105</v>
+        <v>1938</v>
       </c>
       <c r="D18" s="1">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -4152,31 +4279,31 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C19" s="1">
-        <v>1929</v>
+        <v>3105</v>
       </c>
       <c r="D19" s="1">
         <v>98</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>155</v>
+        <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>182</v>
+        <v>80</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -4188,17 +4315,37 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1929</v>
+      </c>
+      <c r="D20" s="1">
+        <v>98</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -4211,34 +4358,34 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="C21" s="1">
-        <v>1974</v>
+        <v>2745</v>
       </c>
       <c r="D21" s="1">
         <v>100</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>105</v>
+        <v>205</v>
       </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -4250,37 +4397,17 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2046</v>
-      </c>
-      <c r="D22" s="1">
-        <v>64</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>119</v>
-      </c>
+    <row r="22" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -4296,31 +4423,31 @@
         <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C23" s="1">
-        <v>3210</v>
+        <v>1974</v>
       </c>
       <c r="D23" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -4337,31 +4464,31 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C24" s="1">
-        <v>2052</v>
+        <v>2046</v>
       </c>
       <c r="D24" s="1">
         <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>118</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -4378,31 +4505,31 @@
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>162</v>
+        <v>120</v>
       </c>
       <c r="C25" s="1">
-        <v>2544</v>
+        <v>3210</v>
       </c>
       <c r="D25" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -4419,31 +4546,31 @@
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1">
-        <v>2284</v>
+        <v>2052</v>
       </c>
       <c r="D26" s="1">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -4460,31 +4587,31 @@
         <v>85</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="C27" s="1">
-        <v>2928</v>
+        <v>2544</v>
       </c>
       <c r="D27" s="1">
         <v>100</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -4501,31 +4628,31 @@
         <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C28" s="1">
-        <v>3039</v>
+        <v>2284</v>
       </c>
       <c r="D28" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>198</v>
+        <v>130</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -4537,17 +4664,37 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2928</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -4560,159 +4707,103 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="C30" s="1">
-        <v>2880</v>
+        <v>3039</v>
       </c>
       <c r="D30" s="1">
         <v>100</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>55</v>
+        <v>197</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
       <c r="C31" s="1">
-        <v>1855</v>
+        <v>2889</v>
       </c>
       <c r="D31" s="1">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>68</v>
+        <v>209</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="1">
-        <v>2341</v>
-      </c>
-      <c r="D32" s="1">
-        <v>98</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>83</v>
-      </c>
+    <row r="32" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -4722,49 +4813,49 @@
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C33" s="1">
-        <v>2361</v>
+        <v>2880</v>
       </c>
       <c r="D33" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>97</v>
+        <v>59</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -4775,49 +4866,49 @@
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1">
-        <v>2584</v>
+        <v>1855</v>
       </c>
       <c r="D34" s="1">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -4828,115 +4919,102 @@
         <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1">
-        <v>3204</v>
+        <v>2341</v>
       </c>
       <c r="D35" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="G35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="J35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="M35" s="1" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>125</v>
+        <v>82</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="Q35" s="1"/>
-      <c r="R35" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S35" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T35" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U35" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="V35" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1">
-        <v>3565</v>
+        <v>2361</v>
       </c>
       <c r="D36" s="1">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="J36" s="1" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>149</v>
+        <v>58</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>150</v>
+        <v>97</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -4947,49 +5025,49 @@
         <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="C37" s="1">
-        <v>2780</v>
+        <v>2584</v>
       </c>
       <c r="D37" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>173</v>
+        <v>110</v>
       </c>
       <c r="O37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -5000,102 +5078,115 @@
         <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1">
-        <v>2683</v>
+        <v>3204</v>
       </c>
       <c r="D38" s="1">
         <v>100</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>154</v>
+        <v>52</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>179</v>
+        <v>76</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>183</v>
+        <v>121</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>184</v>
+        <v>110</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>185</v>
+        <v>123</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
+      <c r="R38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="C39" s="1">
-        <v>3170</v>
+        <v>3565</v>
       </c>
       <c r="D39" s="1">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>76</v>
+        <v>144</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>191</v>
+        <v>149</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>192</v>
+        <v>150</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -5106,138 +5197,268 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="C40" s="1">
-        <v>1910</v>
+        <v>2780</v>
       </c>
       <c r="D40" s="1">
         <v>100</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2683</v>
+      </c>
+      <c r="D41" s="1">
+        <v>100</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="O40" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="P40" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="K41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3170</v>
+      </c>
+      <c r="D42" s="1">
+        <v>98</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1910</v>
+      </c>
+      <c r="D43" s="1">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>206</v>
+      </c>
       <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="R43" s="3" t="s">
+        <v>207</v>
+      </c>
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2860</v>
+      </c>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="R44" s="3" t="s">
+        <v>216</v>
+      </c>
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
@@ -7529,6 +7750,69 @@
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
     </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="K154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+      <c r="N154" s="1"/>
+      <c r="O154" s="1"/>
+      <c r="P154" s="1"/>
+      <c r="Q154" s="1"/>
+      <c r="R154" s="1"/>
+      <c r="S154" s="1"/>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="K155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1"/>
+      <c r="N155" s="1"/>
+      <c r="O155" s="1"/>
+      <c r="P155" s="1"/>
+      <c r="Q155" s="1"/>
+      <c r="R155" s="1"/>
+      <c r="S155" s="1"/>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+      <c r="D156" s="1"/>
+      <c r="E156" s="1"/>
+      <c r="F156" s="1"/>
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="K156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+      <c r="N156" s="1"/>
+      <c r="O156" s="1"/>
+      <c r="P156" s="1"/>
+      <c r="Q156" s="1"/>
+      <c r="R156" s="1"/>
+      <c r="S156" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with Ultimate Squad results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1003" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D570B59-419E-49CF-880E-C95344950288}"/>
+  <xr:revisionPtr revIDLastSave="1026" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04252519-1E76-4495-AA7C-8CF52582EC50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="223">
   <si>
     <t>Type</t>
   </si>
@@ -701,10 +701,10 @@
     <t>Thirty Subs</t>
   </si>
   <si>
-    <t>73/94</t>
-  </si>
-  <si>
     <t>Romandie</t>
+  </si>
+  <si>
+    <t>1h14'08''</t>
   </si>
 </sst>
 </file>
@@ -720,7 +720,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,6 +739,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -752,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -764,6 +770,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1083,7 +1092,7 @@
   <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,16 +1223,18 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>137</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2072,16 +2083,18 @@
       <c r="B42" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>219</v>
+      <c r="C42" s="1">
+        <v>12</v>
       </c>
       <c r="D42" s="1">
         <v>312</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F42" s="1"/>
+      <c r="E42" s="1">
+        <v>33</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="2"/>
     </row>
@@ -3535,7 +3548,7 @@
   <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,7 +3795,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5461,7 +5474,7 @@
       </c>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -5483,22 +5496,54 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C46" s="1">
+        <v>11975</v>
+      </c>
+      <c r="D46" s="1">
+        <v>100</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>

</xml_diff>

<commit_message>
Updated with Romandie and Eschborn-Frankfurt results
</commit_message>
<xml_diff>
--- a/VUT_2022.xlsx
+++ b/VUT_2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75ca376656bd96ab/Documents/Velogames Ultimate Team/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1026" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04252519-1E76-4495-AA7C-8CF52582EC50}"/>
+  <xr:revisionPtr revIDLastSave="1059" documentId="8_{8EEB0EFD-EAA8-439F-9518-58430B5AF5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{044BCCBE-00CF-499D-A49C-02DE6B013758}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{669793BD-1176-416F-A44F-36F75EDCF48C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="231">
   <si>
     <t>Type</t>
   </si>
@@ -705,6 +705,30 @@
   </si>
   <si>
     <t>1h14'08''</t>
+  </si>
+  <si>
+    <t>27''</t>
+  </si>
+  <si>
+    <t>Rohan Dennis</t>
+  </si>
+  <si>
+    <t>Ethan Hayter</t>
+  </si>
+  <si>
+    <t>Gino Maeder</t>
+  </si>
+  <si>
+    <t>Steven Kruijswijk</t>
+  </si>
+  <si>
+    <t>Simon Geschke</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Fernando Gaviria</t>
   </si>
 </sst>
 </file>
@@ -720,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,12 +763,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -758,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -770,9 +788,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1089,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D259F6-3D9A-45EF-8503-BF4EBF3E8F99}">
-  <dimension ref="A1:H185"/>
+  <dimension ref="A1:H186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,10 +1246,14 @@
       <c r="D6" s="1">
         <v>137</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1574,19 +1593,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>229</v>
       </c>
       <c r="C21" s="1">
         <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>39</v>
@@ -1601,16 +1620,16 @@
         <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>6</v>
       </c>
       <c r="D22" s="1">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E22" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>39</v>
@@ -1625,22 +1644,22 @@
         <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C23" s="1">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1">
-        <v>17</v>
-      </c>
-      <c r="F23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -1649,22 +1668,22 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="D24" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1">
-        <v>18</v>
-      </c>
-      <c r="F24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1673,22 +1692,22 @@
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
       </c>
       <c r="D25" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1">
-        <v>23</v>
-      </c>
-      <c r="F25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1697,13 +1716,13 @@
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C26" s="1">
         <v>6</v>
       </c>
       <c r="D26" s="1">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1">
         <v>23</v>
@@ -1712,7 +1731,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1721,22 +1740,22 @@
         <v>85</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C27" s="1">
         <v>6</v>
       </c>
       <c r="D27" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="2"/>
     </row>
@@ -1745,16 +1764,16 @@
         <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C28" s="1">
         <v>6</v>
       </c>
       <c r="D28" s="1">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E28" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>39</v>
@@ -1769,19 +1788,19 @@
         <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C29" s="1">
         <v>6</v>
       </c>
       <c r="D29" s="1">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E29" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
@@ -1790,22 +1809,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="C30" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D30" s="1">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E30" s="1">
-        <v>21</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
@@ -1817,22 +1836,22 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C31" s="1">
         <v>12</v>
       </c>
       <c r="D31" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E31" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="G31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -1841,19 +1860,19 @@
         <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1">
         <v>12</v>
       </c>
       <c r="D32" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E32" s="1">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="G32" s="1">
         <v>2</v>
@@ -1865,19 +1884,19 @@
         <v>49</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1">
         <v>12</v>
       </c>
       <c r="D33" s="1">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E33" s="1">
         <v>19</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G33" s="1">
         <v>2</v>
@@ -1889,19 +1908,19 @@
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C34" s="1">
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="E34" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="G34" s="1">
         <v>2</v>
@@ -1913,22 +1932,22 @@
         <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1">
         <v>12</v>
       </c>
       <c r="D35" s="1">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="G35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -1937,22 +1956,22 @@
         <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C36" s="1">
         <v>12</v>
       </c>
       <c r="D36" s="1">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E36" s="1">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="G36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -1961,22 +1980,22 @@
         <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C37" s="1">
         <v>12</v>
       </c>
       <c r="D37" s="1">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="G37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H37" s="2"/>
     </row>
@@ -1985,22 +2004,22 @@
         <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C38" s="1">
         <v>12</v>
       </c>
       <c r="D38" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E38" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="G38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -2009,22 +2028,22 @@
         <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C39" s="1">
         <v>12</v>
       </c>
       <c r="D39" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E39" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -2033,22 +2052,22 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C40" s="1">
         <v>12</v>
       </c>
       <c r="D40" s="1">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E40" s="1">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>201</v>
+        <v>39</v>
       </c>
       <c r="G40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40" s="2"/>
     </row>
@@ -2057,45 +2076,47 @@
         <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C41" s="1">
         <v>12</v>
       </c>
       <c r="D41" s="1">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E41" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>20</v>
+        <v>201</v>
       </c>
       <c r="G41" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>217</v>
+        <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C42" s="1">
         <v>12</v>
       </c>
       <c r="D42" s="1">
-        <v>312</v>
+        <v>54</v>
       </c>
       <c r="E42" s="1">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,30 +2124,42 @@
         <v>217</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+      <c r="C43" s="1">
+        <v>12</v>
       </c>
       <c r="D43" s="1">
         <v>312</v>
       </c>
       <c r="E43" s="1">
-        <v>94</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D44" s="1">
+        <v>312</v>
+      </c>
+      <c r="E44" s="1">
+        <v>94</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -3538,6 +3571,16 @@
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="1"/>
+      <c r="E186" s="1"/>
+      <c r="F186" s="1"/>
+      <c r="G186" s="1"/>
+      <c r="H186" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3545,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F615EE0-7219-420B-A93D-DB13089F794D}">
-  <dimension ref="A1:V156"/>
+  <dimension ref="A1:V157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3797,17 +3840,39 @@
       <c r="B6" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="C6" s="1">
+        <v>4606</v>
+      </c>
+      <c r="D6" s="1">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -4410,17 +4475,37 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2088</v>
+      </c>
+      <c r="D22" s="1">
+        <v>100</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -4431,37 +4516,17 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1974</v>
-      </c>
-      <c r="D23" s="1">
-        <v>100</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>105</v>
-      </c>
+    <row r="23" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -4477,31 +4542,31 @@
         <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1">
-        <v>2046</v>
+        <v>1974</v>
       </c>
       <c r="D24" s="1">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -4518,31 +4583,31 @@
         <v>85</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C25" s="1">
-        <v>3210</v>
+        <v>2046</v>
       </c>
       <c r="D25" s="1">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -4559,31 +4624,31 @@
         <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C26" s="1">
-        <v>2052</v>
+        <v>3210</v>
       </c>
       <c r="D26" s="1">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -4600,31 +4665,31 @@
         <v>85</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1">
-        <v>2544</v>
+        <v>2052</v>
       </c>
       <c r="D27" s="1">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -4641,31 +4706,31 @@
         <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C28" s="1">
-        <v>2284</v>
+        <v>2544</v>
       </c>
       <c r="D28" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>163</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>165</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -4682,31 +4747,31 @@
         <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1">
-        <v>2928</v>
+        <v>2284</v>
       </c>
       <c r="D29" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>127</v>
+        <v>176</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -4723,31 +4788,31 @@
         <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C30" s="1">
-        <v>3039</v>
+        <v>2928</v>
       </c>
       <c r="D30" s="1">
         <v>100</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>196</v>
+        <v>115</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -4764,10 +4829,10 @@
         <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C31" s="1">
-        <v>2889</v>
+        <v>3039</v>
       </c>
       <c r="D31" s="1">
         <v>100</v>
@@ -4776,19 +4841,19 @@
         <v>126</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>128</v>
+        <v>196</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -4800,17 +4865,37 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2889</v>
+      </c>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -4821,55 +4906,23 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2880</v>
-      </c>
-      <c r="D33" s="1">
-        <v>100</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>61</v>
-      </c>
+    <row r="33" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -4879,49 +4932,49 @@
         <v>49</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C34" s="1">
-        <v>1855</v>
+        <v>2880</v>
       </c>
       <c r="D34" s="1">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="J34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="M34" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
@@ -4932,49 +4985,49 @@
         <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C35" s="1">
-        <v>2341</v>
+        <v>1855</v>
       </c>
       <c r="D35" s="1">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
@@ -4985,49 +5038,49 @@
         <v>49</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1">
-        <v>2361</v>
+        <v>2341</v>
       </c>
       <c r="D36" s="1">
         <v>98</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
@@ -5038,49 +5091,49 @@
         <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1">
-        <v>2584</v>
+        <v>2361</v>
       </c>
       <c r="D37" s="1">
+        <v>98</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="O37" s="1" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
@@ -5091,168 +5144,168 @@
         <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C38" s="1">
-        <v>3204</v>
+        <v>2584</v>
       </c>
       <c r="D38" s="1">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="L38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="P38" s="3" t="s">
-        <v>125</v>
+      <c r="P38" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="Q38" s="1"/>
-      <c r="R38" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="S38" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="T38" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="U38" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="V38" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C39" s="1">
-        <v>3565</v>
+        <v>3204</v>
       </c>
       <c r="D39" s="1">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>152</v>
+        <v>76</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>151</v>
+        <v>123</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
+      <c r="R39" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="V39" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="C40" s="1">
-        <v>2780</v>
+        <v>3565</v>
       </c>
       <c r="D40" s="1">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>168</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -5263,49 +5316,49 @@
         <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C41" s="1">
-        <v>2683</v>
+        <v>2780</v>
       </c>
       <c r="D41" s="1">
         <v>100</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>179</v>
+        <v>79</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>180</v>
+        <v>76</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>37</v>
+        <v>172</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -5316,49 +5369,49 @@
         <v>49</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C42" s="1">
-        <v>3170</v>
+        <v>2683</v>
       </c>
       <c r="D42" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>76</v>
+        <v>182</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>192</v>
+        <v>37</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="N42" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="P42" s="1" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -5369,54 +5422,52 @@
         <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C43" s="1">
-        <v>1910</v>
+        <v>3170</v>
       </c>
       <c r="D43" s="1">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>16</v>
+        <v>193</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>182</v>
+        <v>70</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>203</v>
+        <v>80</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="O43" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>206</v>
+        <v>110</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="Q43" s="1"/>
-      <c r="R43" s="3" t="s">
-        <v>207</v>
-      </c>
+      <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
@@ -5424,147 +5475,181 @@
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C44" s="1">
-        <v>2860</v>
+        <v>1910</v>
       </c>
       <c r="D44" s="1">
         <v>100</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>22</v>
+        <v>202</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>16</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>182</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="L44" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="M44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="N44" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="P44" s="3" t="s">
-        <v>161</v>
+        <v>206</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="1">
+        <v>2860</v>
+      </c>
+      <c r="D45" s="1">
+        <v>100</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="S44" s="1"/>
-    </row>
-    <row r="45" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C46" s="1">
-        <v>11975</v>
-      </c>
-      <c r="D46" s="1">
-        <v>100</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N46" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>191</v>
-      </c>
+    <row r="46" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C47" s="1">
+        <v>11975</v>
+      </c>
+      <c r="D47" s="1">
+        <v>100</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="N47" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
@@ -7858,6 +7943,27 @@
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
     </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="1"/>
+      <c r="E157" s="1"/>
+      <c r="F157" s="1"/>
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
+      <c r="Q157" s="1"/>
+      <c r="R157" s="1"/>
+      <c r="S157" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>